<commit_message>
Add rule submission forms; update dqc_0014 list of elements & rules index
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0014/DQC_0014_ListOfElements.xlsx
+++ b/docs/DQC_US_0014/DQC_0014_ListOfElements.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanyount/Documents/dqc_us_rules/docs/DQC_US_0014/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15040" yWindow="460" windowWidth="36160" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="15045" yWindow="465" windowWidth="36165" windowHeight="19545" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$35</definedName>
+  </definedNames>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
   <si>
     <t>Release Version</t>
   </si>
@@ -345,13 +344,34 @@
   </si>
   <si>
     <t>The number of new shares issued in the conversion of stock in a noncash (or part noncash) transaction. Noncash is defined as transactions during a period that do not result in cash receipts or cash payments in the period. "Part noncash" refers to that portion of the transaction not resulting in cash receipts or cash payments in the period.</t>
+  </si>
+  <si>
+    <t>Fair Value, Measurement with Unobservable Inputs Reconciliation, Liability, Transfers out of Level 3</t>
+  </si>
+  <si>
+    <t>FairValueMeasurementWithUnobservableInputsReconciliationLiabilityTransfersOutOfLevel3</t>
+  </si>
+  <si>
+    <t>Amount of transfers of financial instrument classified as a liability out of level 3 of the fair value hierarchy.</t>
+  </si>
+  <si>
+    <t>RevenueFromContractWithCustomerIncludingAssessedTax</t>
+  </si>
+  <si>
+    <t>RevenueFromContractWithCustomerExcludingAssessedTax</t>
+  </si>
+  <si>
+    <t>Change the filter above to review the full list of elements for DQC_0014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,8 +413,33 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +449,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -424,7 +475,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -447,6 +498,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -509,7 +575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +610,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,34 +787,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="71.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="14.875" style="3" customWidth="1"/>
+    <col min="2" max="4" width="10.875" style="3"/>
+    <col min="5" max="5" width="71.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="9"/>
     <col min="9" max="9" width="150" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="3"/>
+    <col min="10" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -776,15 +843,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" hidden="1">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
+      <c r="B2" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C2" s="10">
+        <v>42736</v>
       </c>
       <c r="D2" s="5">
         <v>2786</v>
@@ -805,15 +872,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="32.25" hidden="1">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
+      <c r="B3" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C3" s="10">
+        <v>42736</v>
       </c>
       <c r="D3" s="5">
         <v>2787</v>
@@ -834,15 +901,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="32.25" hidden="1">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
+      <c r="B4" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C4" s="10">
+        <v>42736</v>
       </c>
       <c r="D4" s="5">
         <v>2788</v>
@@ -863,15 +930,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="32.25" hidden="1">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
+      <c r="B5" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C5" s="10">
+        <v>42736</v>
       </c>
       <c r="D5" s="5">
         <v>2789</v>
@@ -892,15 +959,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18.75" hidden="1">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
+      <c r="B6" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C6" s="10">
+        <v>42736</v>
       </c>
       <c r="D6" s="5">
         <v>2790</v>
@@ -921,15 +988,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="48" hidden="1">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
+      <c r="B7" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C7" s="10">
+        <v>42736</v>
       </c>
       <c r="D7" s="5">
         <v>2791</v>
@@ -950,15 +1017,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="48" hidden="1">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
+      <c r="B8" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C8" s="10">
+        <v>42736</v>
       </c>
       <c r="D8" s="5">
         <v>2792</v>
@@ -979,15 +1046,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="32.25" hidden="1">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
+      <c r="B9" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C9" s="10">
+        <v>42736</v>
       </c>
       <c r="D9" s="5">
         <v>2793</v>
@@ -1008,15 +1075,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="32.25" hidden="1">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
+      <c r="B10" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C10" s="10">
+        <v>42736</v>
       </c>
       <c r="D10" s="5">
         <v>2794</v>
@@ -1037,15 +1104,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="48" hidden="1">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
+      <c r="B11" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C11" s="10">
+        <v>42736</v>
       </c>
       <c r="D11" s="5">
         <v>2795</v>
@@ -1066,15 +1133,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="48" hidden="1">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
+      <c r="B12" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C12" s="10">
+        <v>42736</v>
       </c>
       <c r="D12" s="5">
         <v>2796</v>
@@ -1095,15 +1162,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="48" hidden="1">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
+      <c r="B13" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C13" s="10">
+        <v>42736</v>
       </c>
       <c r="D13" s="5">
         <v>2797</v>
@@ -1124,15 +1191,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="32.25" hidden="1">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
+      <c r="B14" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C14" s="10">
+        <v>42736</v>
       </c>
       <c r="D14" s="5">
         <v>2798</v>
@@ -1153,15 +1220,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="48" hidden="1">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
+      <c r="B15" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C15" s="10">
+        <v>42736</v>
       </c>
       <c r="D15" s="5">
         <v>2799</v>
@@ -1182,15 +1249,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="32.25" hidden="1">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
+      <c r="B16" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C16" s="10">
+        <v>42736</v>
       </c>
       <c r="D16" s="5">
         <v>2800</v>
@@ -1211,15 +1278,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="32.25" hidden="1">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
+      <c r="B17" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C17" s="10">
+        <v>42736</v>
       </c>
       <c r="D17" s="5">
         <v>2801</v>
@@ -1240,15 +1307,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="48" hidden="1">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
+      <c r="B18" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C18" s="10">
+        <v>42736</v>
       </c>
       <c r="D18" s="5">
         <v>2802</v>
@@ -1269,15 +1336,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="48" hidden="1">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
+      <c r="B19" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C19" s="10">
+        <v>42736</v>
       </c>
       <c r="D19" s="5">
         <v>2803</v>
@@ -1298,15 +1365,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="32.25" hidden="1">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
+      <c r="B20" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C20" s="10">
+        <v>42736</v>
       </c>
       <c r="D20" s="5">
         <v>2804</v>
@@ -1327,15 +1394,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="18.75" hidden="1">
       <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
+      <c r="B21" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C21" s="10">
+        <v>42736</v>
       </c>
       <c r="D21" s="5">
         <v>2805</v>
@@ -1356,15 +1423,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="18.75" hidden="1">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
+      <c r="B22" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C22" s="10">
+        <v>42736</v>
       </c>
       <c r="D22" s="5">
         <v>2806</v>
@@ -1385,15 +1452,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="32.25" hidden="1">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
+      <c r="B23" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C23" s="10">
+        <v>42736</v>
       </c>
       <c r="D23" s="5">
         <v>2807</v>
@@ -1414,15 +1481,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="32.25" hidden="1">
       <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
+      <c r="B24" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C24" s="10">
+        <v>42736</v>
       </c>
       <c r="D24" s="5">
         <v>2808</v>
@@ -1443,15 +1510,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="32.25" hidden="1">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>10</v>
+      <c r="B25" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C25" s="10">
+        <v>42736</v>
       </c>
       <c r="D25" s="5">
         <v>2809</v>
@@ -1472,15 +1539,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>10</v>
+      <c r="B26" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C26" s="10">
+        <v>42736</v>
       </c>
       <c r="D26" s="5">
         <v>3003</v>
@@ -1501,15 +1568,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
+      <c r="B27" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C27" s="10">
+        <v>42736</v>
       </c>
       <c r="D27" s="5">
         <v>3004</v>
@@ -1530,15 +1597,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
+      <c r="B28" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C28" s="10">
+        <v>42736</v>
       </c>
       <c r="D28" s="5">
         <v>3005</v>
@@ -1557,15 +1624,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>10</v>
+      <c r="B29" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C29" s="10">
+        <v>42736</v>
       </c>
       <c r="D29" s="5">
         <v>3006</v>
@@ -1586,15 +1653,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>10</v>
+      <c r="B30" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C30" s="10">
+        <v>42736</v>
       </c>
       <c r="D30" s="5">
         <v>3007</v>
@@ -1615,15 +1682,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>10</v>
+      <c r="B31" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C31" s="10">
+        <v>42736</v>
       </c>
       <c r="D31" s="5">
         <v>3008</v>
@@ -1644,15 +1711,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>10</v>
+      <c r="B32" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C32" s="10">
+        <v>42736</v>
       </c>
       <c r="D32" s="5">
         <v>3009</v>
@@ -1671,7 +1738,109 @@
         <v>105</v>
       </c>
     </row>
+    <row r="33" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A33" s="15">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="12">
+        <v>3096</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A34" s="15">
+        <v>7</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="12">
+        <v>7651</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A35" s="15">
+        <v>7</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="12">
+        <v>7652</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="14"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I35">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="7.0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add rule submission forms for Committee review - v7 public exposure (#323)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0014/DQC_0014_ListOfElements.xlsx
+++ b/docs/DQC_US_0014/DQC_0014_ListOfElements.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanyount/Documents/dqc_us_rules/docs/DQC_US_0014/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15040" yWindow="460" windowWidth="36160" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="15045" yWindow="465" windowWidth="36165" windowHeight="19545" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$35</definedName>
+  </definedNames>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
   <si>
     <t>Release Version</t>
   </si>
@@ -345,13 +344,34 @@
   </si>
   <si>
     <t>The number of new shares issued in the conversion of stock in a noncash (or part noncash) transaction. Noncash is defined as transactions during a period that do not result in cash receipts or cash payments in the period. "Part noncash" refers to that portion of the transaction not resulting in cash receipts or cash payments in the period.</t>
+  </si>
+  <si>
+    <t>Fair Value, Measurement with Unobservable Inputs Reconciliation, Liability, Transfers out of Level 3</t>
+  </si>
+  <si>
+    <t>FairValueMeasurementWithUnobservableInputsReconciliationLiabilityTransfersOutOfLevel3</t>
+  </si>
+  <si>
+    <t>Amount of transfers of financial instrument classified as a liability out of level 3 of the fair value hierarchy.</t>
+  </si>
+  <si>
+    <t>RevenueFromContractWithCustomerIncludingAssessedTax</t>
+  </si>
+  <si>
+    <t>RevenueFromContractWithCustomerExcludingAssessedTax</t>
+  </si>
+  <si>
+    <t>Change the filter above to review the full list of elements for DQC_0014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,8 +413,33 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +449,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -424,7 +475,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -447,6 +498,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -509,7 +575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +610,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,34 +787,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="71.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="14.875" style="3" customWidth="1"/>
+    <col min="2" max="4" width="10.875" style="3"/>
+    <col min="5" max="5" width="71.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="9"/>
     <col min="9" max="9" width="150" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="3"/>
+    <col min="10" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -776,15 +843,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" hidden="1">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
+      <c r="B2" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C2" s="10">
+        <v>42736</v>
       </c>
       <c r="D2" s="5">
         <v>2786</v>
@@ -805,15 +872,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="32.25" hidden="1">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
+      <c r="B3" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C3" s="10">
+        <v>42736</v>
       </c>
       <c r="D3" s="5">
         <v>2787</v>
@@ -834,15 +901,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="32.25" hidden="1">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
+      <c r="B4" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C4" s="10">
+        <v>42736</v>
       </c>
       <c r="D4" s="5">
         <v>2788</v>
@@ -863,15 +930,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="32.25" hidden="1">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
+      <c r="B5" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C5" s="10">
+        <v>42736</v>
       </c>
       <c r="D5" s="5">
         <v>2789</v>
@@ -892,15 +959,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18.75" hidden="1">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
+      <c r="B6" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C6" s="10">
+        <v>42736</v>
       </c>
       <c r="D6" s="5">
         <v>2790</v>
@@ -921,15 +988,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="48" hidden="1">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
+      <c r="B7" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C7" s="10">
+        <v>42736</v>
       </c>
       <c r="D7" s="5">
         <v>2791</v>
@@ -950,15 +1017,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="48" hidden="1">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
+      <c r="B8" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C8" s="10">
+        <v>42736</v>
       </c>
       <c r="D8" s="5">
         <v>2792</v>
@@ -979,15 +1046,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="32.25" hidden="1">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
+      <c r="B9" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C9" s="10">
+        <v>42736</v>
       </c>
       <c r="D9" s="5">
         <v>2793</v>
@@ -1008,15 +1075,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="32.25" hidden="1">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
+      <c r="B10" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C10" s="10">
+        <v>42736</v>
       </c>
       <c r="D10" s="5">
         <v>2794</v>
@@ -1037,15 +1104,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="48" hidden="1">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
+      <c r="B11" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C11" s="10">
+        <v>42736</v>
       </c>
       <c r="D11" s="5">
         <v>2795</v>
@@ -1066,15 +1133,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="48" hidden="1">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
+      <c r="B12" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C12" s="10">
+        <v>42736</v>
       </c>
       <c r="D12" s="5">
         <v>2796</v>
@@ -1095,15 +1162,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="48" hidden="1">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
+      <c r="B13" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C13" s="10">
+        <v>42736</v>
       </c>
       <c r="D13" s="5">
         <v>2797</v>
@@ -1124,15 +1191,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="32.25" hidden="1">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
+      <c r="B14" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C14" s="10">
+        <v>42736</v>
       </c>
       <c r="D14" s="5">
         <v>2798</v>
@@ -1153,15 +1220,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="48" hidden="1">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
+      <c r="B15" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C15" s="10">
+        <v>42736</v>
       </c>
       <c r="D15" s="5">
         <v>2799</v>
@@ -1182,15 +1249,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="32.25" hidden="1">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
+      <c r="B16" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C16" s="10">
+        <v>42736</v>
       </c>
       <c r="D16" s="5">
         <v>2800</v>
@@ -1211,15 +1278,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="32.25" hidden="1">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
+      <c r="B17" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C17" s="10">
+        <v>42736</v>
       </c>
       <c r="D17" s="5">
         <v>2801</v>
@@ -1240,15 +1307,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="48" hidden="1">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
+      <c r="B18" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C18" s="10">
+        <v>42736</v>
       </c>
       <c r="D18" s="5">
         <v>2802</v>
@@ -1269,15 +1336,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="48" hidden="1">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
+      <c r="B19" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C19" s="10">
+        <v>42736</v>
       </c>
       <c r="D19" s="5">
         <v>2803</v>
@@ -1298,15 +1365,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="32.25" hidden="1">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
+      <c r="B20" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C20" s="10">
+        <v>42736</v>
       </c>
       <c r="D20" s="5">
         <v>2804</v>
@@ -1327,15 +1394,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="18.75" hidden="1">
       <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
+      <c r="B21" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C21" s="10">
+        <v>42736</v>
       </c>
       <c r="D21" s="5">
         <v>2805</v>
@@ -1356,15 +1423,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="18.75" hidden="1">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
+      <c r="B22" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C22" s="10">
+        <v>42736</v>
       </c>
       <c r="D22" s="5">
         <v>2806</v>
@@ -1385,15 +1452,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="32.25" hidden="1">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
+      <c r="B23" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C23" s="10">
+        <v>42736</v>
       </c>
       <c r="D23" s="5">
         <v>2807</v>
@@ -1414,15 +1481,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="32.25" hidden="1">
       <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
+      <c r="B24" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C24" s="10">
+        <v>42736</v>
       </c>
       <c r="D24" s="5">
         <v>2808</v>
@@ -1443,15 +1510,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="32.25" hidden="1">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>10</v>
+      <c r="B25" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C25" s="10">
+        <v>42736</v>
       </c>
       <c r="D25" s="5">
         <v>2809</v>
@@ -1472,15 +1539,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>10</v>
+      <c r="B26" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C26" s="10">
+        <v>42736</v>
       </c>
       <c r="D26" s="5">
         <v>3003</v>
@@ -1501,15 +1568,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
+      <c r="B27" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C27" s="10">
+        <v>42736</v>
       </c>
       <c r="D27" s="5">
         <v>3004</v>
@@ -1530,15 +1597,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
+      <c r="B28" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C28" s="10">
+        <v>42736</v>
       </c>
       <c r="D28" s="5">
         <v>3005</v>
@@ -1557,15 +1624,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>10</v>
+      <c r="B29" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C29" s="10">
+        <v>42736</v>
       </c>
       <c r="D29" s="5">
         <v>3006</v>
@@ -1586,15 +1653,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>10</v>
+      <c r="B30" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C30" s="10">
+        <v>42736</v>
       </c>
       <c r="D30" s="5">
         <v>3007</v>
@@ -1615,15 +1682,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>10</v>
+      <c r="B31" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C31" s="10">
+        <v>42736</v>
       </c>
       <c r="D31" s="5">
         <v>3008</v>
@@ -1644,15 +1711,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>10</v>
+      <c r="B32" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C32" s="10">
+        <v>42736</v>
       </c>
       <c r="D32" s="5">
         <v>3009</v>
@@ -1671,7 +1738,109 @@
         <v>105</v>
       </c>
     </row>
+    <row r="33" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A33" s="15">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="12">
+        <v>3096</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A34" s="15">
+        <v>7</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="12">
+        <v>7651</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A35" s="15">
+        <v>7</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="12">
+        <v>7652</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="14"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I35">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="7.0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update with v7.0.1 dqc_us_rules (#4)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0014/DQC_0014_ListOfElements.xlsx
+++ b/docs/DQC_US_0014/DQC_0014_ListOfElements.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanyount/Documents/dqc_us_rules/docs/DQC_US_0014/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15040" yWindow="460" windowWidth="36160" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="15045" yWindow="465" windowWidth="36165" windowHeight="19545" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$35</definedName>
+  </definedNames>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
   <si>
     <t>Release Version</t>
   </si>
@@ -345,13 +344,34 @@
   </si>
   <si>
     <t>The number of new shares issued in the conversion of stock in a noncash (or part noncash) transaction. Noncash is defined as transactions during a period that do not result in cash receipts or cash payments in the period. "Part noncash" refers to that portion of the transaction not resulting in cash receipts or cash payments in the period.</t>
+  </si>
+  <si>
+    <t>Fair Value, Measurement with Unobservable Inputs Reconciliation, Liability, Transfers out of Level 3</t>
+  </si>
+  <si>
+    <t>FairValueMeasurementWithUnobservableInputsReconciliationLiabilityTransfersOutOfLevel3</t>
+  </si>
+  <si>
+    <t>Amount of transfers of financial instrument classified as a liability out of level 3 of the fair value hierarchy.</t>
+  </si>
+  <si>
+    <t>RevenueFromContractWithCustomerIncludingAssessedTax</t>
+  </si>
+  <si>
+    <t>RevenueFromContractWithCustomerExcludingAssessedTax</t>
+  </si>
+  <si>
+    <t>Change the filter above to review the full list of elements for DQC_0014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,8 +413,33 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +449,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -424,7 +475,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -447,6 +498,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -509,7 +575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +610,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,34 +787,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="71.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="14.875" style="3" customWidth="1"/>
+    <col min="2" max="4" width="10.875" style="3"/>
+    <col min="5" max="5" width="71.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="9"/>
     <col min="9" max="9" width="150" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="3"/>
+    <col min="10" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -776,15 +843,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" hidden="1">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
+      <c r="B2" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C2" s="10">
+        <v>42736</v>
       </c>
       <c r="D2" s="5">
         <v>2786</v>
@@ -805,15 +872,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="32.25" hidden="1">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
+      <c r="B3" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C3" s="10">
+        <v>42736</v>
       </c>
       <c r="D3" s="5">
         <v>2787</v>
@@ -834,15 +901,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="32.25" hidden="1">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
+      <c r="B4" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C4" s="10">
+        <v>42736</v>
       </c>
       <c r="D4" s="5">
         <v>2788</v>
@@ -863,15 +930,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="32.25" hidden="1">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
+      <c r="B5" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C5" s="10">
+        <v>42736</v>
       </c>
       <c r="D5" s="5">
         <v>2789</v>
@@ -892,15 +959,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18.75" hidden="1">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
+      <c r="B6" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C6" s="10">
+        <v>42736</v>
       </c>
       <c r="D6" s="5">
         <v>2790</v>
@@ -921,15 +988,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="48" hidden="1">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
+      <c r="B7" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C7" s="10">
+        <v>42736</v>
       </c>
       <c r="D7" s="5">
         <v>2791</v>
@@ -950,15 +1017,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="48" hidden="1">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
+      <c r="B8" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C8" s="10">
+        <v>42736</v>
       </c>
       <c r="D8" s="5">
         <v>2792</v>
@@ -979,15 +1046,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="32.25" hidden="1">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
+      <c r="B9" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C9" s="10">
+        <v>42736</v>
       </c>
       <c r="D9" s="5">
         <v>2793</v>
@@ -1008,15 +1075,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="32.25" hidden="1">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
+      <c r="B10" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C10" s="10">
+        <v>42736</v>
       </c>
       <c r="D10" s="5">
         <v>2794</v>
@@ -1037,15 +1104,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="48" hidden="1">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
+      <c r="B11" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C11" s="10">
+        <v>42736</v>
       </c>
       <c r="D11" s="5">
         <v>2795</v>
@@ -1066,15 +1133,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="48" hidden="1">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
+      <c r="B12" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C12" s="10">
+        <v>42736</v>
       </c>
       <c r="D12" s="5">
         <v>2796</v>
@@ -1095,15 +1162,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="48" hidden="1">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
+      <c r="B13" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C13" s="10">
+        <v>42736</v>
       </c>
       <c r="D13" s="5">
         <v>2797</v>
@@ -1124,15 +1191,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="32.25" hidden="1">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
+      <c r="B14" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C14" s="10">
+        <v>42736</v>
       </c>
       <c r="D14" s="5">
         <v>2798</v>
@@ -1153,15 +1220,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="48" hidden="1">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
+      <c r="B15" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C15" s="10">
+        <v>42736</v>
       </c>
       <c r="D15" s="5">
         <v>2799</v>
@@ -1182,15 +1249,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="32.25" hidden="1">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
+      <c r="B16" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C16" s="10">
+        <v>42736</v>
       </c>
       <c r="D16" s="5">
         <v>2800</v>
@@ -1211,15 +1278,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="32.25" hidden="1">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
+      <c r="B17" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C17" s="10">
+        <v>42736</v>
       </c>
       <c r="D17" s="5">
         <v>2801</v>
@@ -1240,15 +1307,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="48" hidden="1">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
+      <c r="B18" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C18" s="10">
+        <v>42736</v>
       </c>
       <c r="D18" s="5">
         <v>2802</v>
@@ -1269,15 +1336,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="48" hidden="1">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
+      <c r="B19" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C19" s="10">
+        <v>42736</v>
       </c>
       <c r="D19" s="5">
         <v>2803</v>
@@ -1298,15 +1365,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="32.25" hidden="1">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
+      <c r="B20" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C20" s="10">
+        <v>42736</v>
       </c>
       <c r="D20" s="5">
         <v>2804</v>
@@ -1327,15 +1394,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="18.75" hidden="1">
       <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
+      <c r="B21" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C21" s="10">
+        <v>42736</v>
       </c>
       <c r="D21" s="5">
         <v>2805</v>
@@ -1356,15 +1423,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="18.75" hidden="1">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
+      <c r="B22" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C22" s="10">
+        <v>42736</v>
       </c>
       <c r="D22" s="5">
         <v>2806</v>
@@ -1385,15 +1452,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="32.25" hidden="1">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
+      <c r="B23" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C23" s="10">
+        <v>42736</v>
       </c>
       <c r="D23" s="5">
         <v>2807</v>
@@ -1414,15 +1481,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="32.25" hidden="1">
       <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
+      <c r="B24" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C24" s="10">
+        <v>42736</v>
       </c>
       <c r="D24" s="5">
         <v>2808</v>
@@ -1443,15 +1510,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="32.25" hidden="1">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>10</v>
+      <c r="B25" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C25" s="10">
+        <v>42736</v>
       </c>
       <c r="D25" s="5">
         <v>2809</v>
@@ -1472,15 +1539,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>10</v>
+      <c r="B26" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C26" s="10">
+        <v>42736</v>
       </c>
       <c r="D26" s="5">
         <v>3003</v>
@@ -1501,15 +1568,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
+      <c r="B27" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C27" s="10">
+        <v>42736</v>
       </c>
       <c r="D27" s="5">
         <v>3004</v>
@@ -1530,15 +1597,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
+      <c r="B28" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C28" s="10">
+        <v>42736</v>
       </c>
       <c r="D28" s="5">
         <v>3005</v>
@@ -1557,15 +1624,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>10</v>
+      <c r="B29" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C29" s="10">
+        <v>42736</v>
       </c>
       <c r="D29" s="5">
         <v>3006</v>
@@ -1586,15 +1653,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>10</v>
+      <c r="B30" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C30" s="10">
+        <v>42736</v>
       </c>
       <c r="D30" s="5">
         <v>3007</v>
@@ -1615,15 +1682,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>10</v>
+      <c r="B31" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C31" s="10">
+        <v>42736</v>
       </c>
       <c r="D31" s="5">
         <v>3008</v>
@@ -1644,15 +1711,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="5" customFormat="1" ht="18.75" hidden="1">
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>10</v>
+      <c r="B32" s="10">
+        <v>42642</v>
+      </c>
+      <c r="C32" s="10">
+        <v>42736</v>
       </c>
       <c r="D32" s="5">
         <v>3009</v>
@@ -1671,7 +1738,109 @@
         <v>105</v>
       </c>
     </row>
+    <row r="33" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A33" s="15">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="12">
+        <v>3096</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A34" s="15">
+        <v>7</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="12">
+        <v>7651</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" s="13" customFormat="1" ht="18.75">
+      <c r="A35" s="15">
+        <v>7</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="12">
+        <v>7652</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="14"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I35">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="7.0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>